<commit_message>
Updated code next demo with email approval
</commit_message>
<xml_diff>
--- a/VereitSuite/VereitApp/testEnvironmentData/databidcreation.xlsx
+++ b/VereitSuite/VereitApp/testEnvironmentData/databidcreation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Bid Name</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Approved</t>
+  </si>
+  <si>
+    <t>1,00,001</t>
   </si>
 </sst>
 </file>
@@ -378,7 +381,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,8 +423,8 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1">
-        <v>10000</v>
+      <c r="D2" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>

</xml_diff>